<commit_message>
updated some minor improvements
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sachi\Documents\Projects\alumni-smvdu-webapp\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sachi\OneDrive\Documents\Projects\alumni-smvdu-webapp\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B95DCF5-2A88-45B8-820D-CEF74107DFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7670A3D-74CE-4223-AFB5-99B33B397EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="1" r:id="rId1"/>
     <sheet name="2024" sheetId="2" r:id="rId2"/>
     <sheet name="2025" sheetId="3" r:id="rId3"/>
-    <sheet name="2026" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="326">
   <si>
     <t>Sno</t>
   </si>
@@ -1000,64 +999,7 @@
     <t>21BCS091</t>
   </si>
   <si>
-    <t>Sachin Anand</t>
-  </si>
-  <si>
-    <t>sachinanand4703@gmail.com</t>
-  </si>
-  <si>
-    <t>8493968619</t>
-  </si>
-  <si>
-    <t>22bcs070</t>
-  </si>
-  <si>
-    <t>Undergraduate (B.Tech)</t>
-  </si>
-  <si>
-    <t>Engineer</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>tokyo</t>
-  </si>
-  <si>
-    <t>tokyo, japan</t>
-  </si>
-  <si>
-    <t>adf</t>
-  </si>
-  <si>
-    <t>fdsa</t>
-  </si>
-  <si>
-    <t>asdfasfd</t>
-  </si>
-  <si>
-    <t>/uploads/alumni/WhatsApp Image 2025-07-31 at 23.30.54_fa8d56cd_2025-07-31T18-58-35-552Z_kn3lrs.jpg</t>
-  </si>
-  <si>
-    <t>/uploads/alumni/1729884727154.jpg</t>
-  </si>
-  <si>
     <t>/uploads/alumni/1660639306910.jpg</t>
-  </si>
-  <si>
-    <t>/uploads/alumni/1718483964303.jpg</t>
-  </si>
-  <si>
-    <t>/uploads/alumni/1626874685626.jpg</t>
-  </si>
-  <si>
-    <t>/uploads/alumni/1747939255648.jpg</t>
-  </si>
-  <si>
-    <t>/uploads/alumni/1720011578203.jpg</t>
-  </si>
-  <si>
-    <t>/uploads/alumni/1702405973799.jpg</t>
   </si>
 </sst>
 </file>
@@ -1436,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1648,7 +1590,7 @@
         <v>30</v>
       </c>
       <c r="Q7" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1676,9 +1618,6 @@
       <c r="O8" t="s">
         <v>26</v>
       </c>
-      <c r="Q8" t="s">
-        <v>339</v>
-      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1705,9 +1644,6 @@
       <c r="O9" t="s">
         <v>31</v>
       </c>
-      <c r="Q9" t="s">
-        <v>339</v>
-      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1812,9 +1748,6 @@
       <c r="O13" t="s">
         <v>21</v>
       </c>
-      <c r="Q13" t="s">
-        <v>340</v>
-      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1841,9 +1774,6 @@
       <c r="O14" t="s">
         <v>26</v>
       </c>
-      <c r="Q14" t="s">
-        <v>340</v>
-      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1897,7 +1827,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1923,7 +1853,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1949,7 +1879,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1975,7 +1905,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2000,11 +1930,8 @@
       <c r="O20" t="s">
         <v>34</v>
       </c>
-      <c r="Q20" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2029,11 +1956,8 @@
       <c r="O21" t="s">
         <v>25</v>
       </c>
-      <c r="Q21" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2059,7 +1983,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2084,11 +2008,8 @@
       <c r="O23" t="s">
         <v>50</v>
       </c>
-      <c r="Q23" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2114,7 +2035,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2140,7 +2061,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2165,11 +2086,8 @@
       <c r="O26" t="s">
         <v>22</v>
       </c>
-      <c r="Q26" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2194,11 +2112,8 @@
       <c r="O27" t="s">
         <v>50</v>
       </c>
-      <c r="Q27" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2223,11 +2138,8 @@
       <c r="O28" t="s">
         <v>34</v>
       </c>
-      <c r="Q28" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2252,11 +2164,8 @@
       <c r="O29" t="s">
         <v>26</v>
       </c>
-      <c r="Q29" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2281,11 +2190,8 @@
       <c r="O30" t="s">
         <v>31</v>
       </c>
-      <c r="Q30" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2311,7 +2217,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2337,7 +2243,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2363,7 +2269,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2388,11 +2294,8 @@
       <c r="O34" t="s">
         <v>25</v>
       </c>
-      <c r="Q34" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2418,7 +2321,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2444,7 +2347,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2470,7 +2373,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2496,7 +2399,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2522,7 +2425,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2548,7 +2451,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2574,7 +2477,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2600,7 +2503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2626,7 +2529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2652,7 +2555,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2678,7 +2581,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2704,7 +2607,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2730,7 +2633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2756,7 +2659,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2782,7 +2685,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2808,7 +2711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2834,7 +2737,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2860,7 +2763,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2886,7 +2789,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2912,7 +2815,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2937,11 +2840,8 @@
       <c r="O55" t="s">
         <v>21</v>
       </c>
-      <c r="Q55" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2966,11 +2866,8 @@
       <c r="O56" t="s">
         <v>30</v>
       </c>
-      <c r="Q56" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2995,11 +2892,8 @@
       <c r="O57" t="s">
         <v>26</v>
       </c>
-      <c r="Q57" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3025,7 +2919,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3051,7 +2945,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3077,7 +2971,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3103,7 +2997,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3129,7 +3023,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3155,7 +3049,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4675,7 +4569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5573,7 +5467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -6909,122 +6803,4 @@
     <ignoredError sqref="A1:Q45" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" t="s">
-        <v>326</v>
-      </c>
-      <c r="D2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E2" t="s">
-        <v>328</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>329</v>
-      </c>
-      <c r="I2" t="s">
-        <v>330</v>
-      </c>
-      <c r="J2" t="s">
-        <v>331</v>
-      </c>
-      <c r="K2" t="s">
-        <v>332</v>
-      </c>
-      <c r="L2" t="s">
-        <v>333</v>
-      </c>
-      <c r="M2" t="s">
-        <v>334</v>
-      </c>
-      <c r="N2" t="s">
-        <v>335</v>
-      </c>
-      <c r="O2" t="s">
-        <v>336</v>
-      </c>
-      <c r="P2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:P1 A2:O2" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>